<commit_message>
1 and 2 TC RF
</commit_message>
<xml_diff>
--- a/RobotFramework_HW/TestCasesRF.xlsx
+++ b/RobotFramework_HW/TestCasesRF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastasiya_Viktarovi\Documents\GitHub\Data-Quality-Engineering-Mentoring-Program-Intermediate-Level-9\RobotFramework_HW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B45386F-2606-4E88-89BC-A5D022D48C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4874EC53-4176-44ED-ABFB-D401632B49AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,9 +542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>